<commit_message>
Adapted outliers and demografics to new Lui read-in
</commit_message>
<xml_diff>
--- a/D_Exploratory_Analyses/B_Outlier_Search/Outlier_Subject_Checks.xlsx
+++ b/D_Exploratory_Analyses/B_Outlier_Search/Outlier_Subject_Checks.xlsx
@@ -96,9 +96,6 @@
     <t>huber_17'</t>
   </si>
   <si>
-    <t>huber_19'</t>
-  </si>
-  <si>
     <t>huber_28'</t>
   </si>
   <si>
@@ -343,6 +340,9 @@
   </si>
   <si>
     <t>wrobel_42'</t>
+  </si>
+  <si>
+    <t>lui28</t>
   </si>
 </sst>
 </file>
@@ -431,8 +431,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="575">
+  <cellStyleXfs count="577">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1027,7 +1029,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="575">
+  <cellStyles count="577">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -1315,6 +1317,7 @@
     <cellStyle name="Besuchter Link" xfId="570" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="572" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="574" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="576" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -1602,6 +1605,7 @@
     <cellStyle name="Link" xfId="569" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="571" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="573" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="575" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1933,8 +1937,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1952,13 +1956,13 @@
         <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G2" s="1"/>
     </row>
@@ -1973,10 +1977,10 @@
         <v>16</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -1993,10 +1997,10 @@
         <v>17</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -2010,13 +2014,13 @@
         <v>3</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -2033,10 +2037,10 @@
         <v>8</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G6" s="10"/>
       <c r="H6" s="10"/>
@@ -2053,13 +2057,13 @@
         <v>6</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G7" s="10"/>
       <c r="H7" s="10"/>
@@ -2079,10 +2083,10 @@
         <v>12</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G8" s="10"/>
       <c r="H8" s="10"/>
@@ -2096,10 +2100,10 @@
         <v>13</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G9" s="10"/>
       <c r="H9" s="10"/>
@@ -2113,10 +2117,10 @@
         <v>14</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G10" s="10"/>
       <c r="H10" s="10"/>
@@ -2130,10 +2134,10 @@
         <v>15</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G11" s="10"/>
       <c r="H11" s="10"/>
@@ -2141,19 +2145,19 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C12" s="10">
         <v>11</v>
       </c>
       <c r="D12" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="E12" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="E12" s="9" t="s">
-        <v>75</v>
-      </c>
       <c r="F12" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G12" s="10"/>
       <c r="H12" s="10"/>
@@ -2161,7 +2165,7 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C13" s="10">
         <v>12</v>
@@ -2170,10 +2174,10 @@
         <v>18</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G13" s="10"/>
       <c r="H13" s="10"/>
@@ -2181,7 +2185,7 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C14">
         <v>13</v>
@@ -2190,10 +2194,10 @@
         <v>19</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G14" s="10"/>
       <c r="H14" s="10"/>
@@ -2207,10 +2211,10 @@
         <v>20</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G15" s="10"/>
       <c r="H15" s="10"/>
@@ -2224,10 +2228,10 @@
         <v>21</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G16" s="10"/>
       <c r="H16" s="10"/>
@@ -2241,10 +2245,10 @@
         <v>22</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="3:9">
@@ -2255,38 +2259,38 @@
         <v>24</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="3:9">
-      <c r="C19" s="10">
-        <v>18</v>
+      <c r="C19">
+        <v>19</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="3:9">
       <c r="C20">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E20" s="15" t="s">
-        <v>70</v>
+      <c r="E20" t="s">
+        <v>79</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G20" s="10"/>
       <c r="H20" s="10"/>
@@ -2294,33 +2298,33 @@
     </row>
     <row r="21" spans="3:9">
       <c r="C21">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>28</v>
       </c>
       <c r="E21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G21" s="10"/>
       <c r="H21" s="10"/>
       <c r="I21" s="10"/>
     </row>
     <row r="22" spans="3:9">
-      <c r="C22">
-        <v>21</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E22" t="s">
+      <c r="C22" s="10">
+        <v>22</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E22" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="F22" s="15" t="s">
-        <v>68</v>
+      <c r="F22" s="16" t="s">
+        <v>67</v>
       </c>
       <c r="G22" s="10"/>
       <c r="H22" s="10"/>
@@ -2328,33 +2332,31 @@
     </row>
     <row r="23" spans="3:9">
       <c r="C23" s="10">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="E23" s="14" t="s">
-        <v>81</v>
+      <c r="E23" s="16" t="s">
+        <v>83</v>
       </c>
       <c r="F23" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G23" s="10"/>
       <c r="H23" s="10"/>
       <c r="I23" s="10"/>
     </row>
     <row r="24" spans="3:9">
-      <c r="C24" s="10">
-        <v>23</v>
-      </c>
+      <c r="C24" s="10"/>
       <c r="D24" s="4" t="s">
-        <v>83</v>
+        <v>107</v>
       </c>
       <c r="E24" s="16" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="F24" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G24" s="10"/>
       <c r="H24" s="10"/>
@@ -2365,13 +2367,13 @@
         <v>24</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="26" spans="3:9">
@@ -2379,13 +2381,13 @@
         <v>25</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="27" spans="3:9">
@@ -2393,13 +2395,13 @@
         <v>26</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="28" spans="3:9">
@@ -2407,13 +2409,13 @@
         <v>27</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="29" spans="3:9">
@@ -2421,13 +2423,13 @@
         <v>28</v>
       </c>
       <c r="D29" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E29" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="E29" s="10" t="s">
-        <v>87</v>
-      </c>
       <c r="F29" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="30" spans="3:9">
@@ -2435,13 +2437,13 @@
         <v>29</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="31" spans="3:9">
@@ -2449,13 +2451,13 @@
         <v>30</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="32" spans="3:9">
@@ -2463,13 +2465,13 @@
         <v>31</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33" spans="3:6">
@@ -2477,13 +2479,13 @@
         <v>32</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F33" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="34" spans="3:6">
@@ -2491,13 +2493,13 @@
         <v>33</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E34" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="35" spans="3:6">
@@ -2505,13 +2507,13 @@
         <v>34</v>
       </c>
       <c r="D35" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="E35" t="s">
         <v>90</v>
       </c>
-      <c r="E35" t="s">
-        <v>91</v>
-      </c>
       <c r="F35" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="36" spans="3:6">
@@ -2519,13 +2521,13 @@
         <v>35</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E36" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F36" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="37" spans="3:6">
@@ -2533,13 +2535,13 @@
         <v>36</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F37" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="38" spans="3:6">
@@ -2547,13 +2549,13 @@
         <v>37</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F38" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="39" spans="3:6">
@@ -2561,13 +2563,13 @@
         <v>38</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E39" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F39" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="40" spans="3:6">
@@ -2575,13 +2577,13 @@
         <v>39</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E40" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F40" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="41" spans="3:6">
@@ -2589,13 +2591,13 @@
         <v>40</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E41" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F41" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="42" spans="3:6">
@@ -2603,13 +2605,13 @@
         <v>41</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F42" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="43" spans="3:6">
@@ -2617,13 +2619,13 @@
         <v>42</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E43" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F43" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="44" spans="3:6">
@@ -2631,13 +2633,13 @@
         <v>43</v>
       </c>
       <c r="D44" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="E44" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="E44" s="10" t="s">
-        <v>96</v>
-      </c>
       <c r="F44" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="45" spans="3:6">
@@ -2645,13 +2647,13 @@
         <v>44</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E45" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F45" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="46" spans="3:6">
@@ -2659,13 +2661,13 @@
         <v>45</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E46" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F46" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="47" spans="3:6">
@@ -2673,13 +2675,13 @@
         <v>46</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E47" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F47" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="48" spans="3:6">
@@ -2687,13 +2689,13 @@
         <v>47</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E48" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F48" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="49" spans="3:7">
@@ -2701,13 +2703,13 @@
         <v>48</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E49" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F49" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="50" spans="3:7">
@@ -2715,13 +2717,13 @@
         <v>49</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E50" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F50" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="51" spans="3:7">
@@ -2732,7 +2734,7 @@
         <v>9</v>
       </c>
       <c r="E51" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F51" s="10" t="s">
         <v>7</v>
@@ -2743,16 +2745,16 @@
         <v>54</v>
       </c>
       <c r="D52" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E52" s="10" t="s">
         <v>39</v>
-      </c>
-      <c r="E52" s="10" t="s">
-        <v>40</v>
       </c>
       <c r="F52" s="10" t="s">
         <v>7</v>
       </c>
       <c r="G52" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="53" spans="3:7">
@@ -2760,16 +2762,16 @@
         <v>55</v>
       </c>
       <c r="D53" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E53" s="10" t="s">
         <v>71</v>
-      </c>
-      <c r="E53" s="10" t="s">
-        <v>72</v>
       </c>
       <c r="F53" s="10" t="s">
         <v>7</v>
       </c>
       <c r="G53" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="54" spans="3:7">
@@ -2780,13 +2782,13 @@
         <v>10</v>
       </c>
       <c r="E54" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F54" s="10" t="s">
         <v>7</v>
       </c>
       <c r="G54" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="55" spans="3:7">
@@ -2797,13 +2799,13 @@
         <v>11</v>
       </c>
       <c r="E55" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F55" s="10" t="s">
         <v>7</v>
       </c>
       <c r="G55" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="56" spans="3:7">
@@ -2811,16 +2813,16 @@
         <v>58</v>
       </c>
       <c r="D56" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E56" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F56" s="10" t="s">
         <v>7</v>
       </c>
       <c r="G56" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="57" spans="3:7">
@@ -2828,16 +2830,16 @@
         <v>59</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E57" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F57" s="10" t="s">
         <v>7</v>
       </c>
       <c r="G57" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="58" spans="3:7">
@@ -2848,13 +2850,13 @@
         <v>23</v>
       </c>
       <c r="E58" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F58" s="10" t="s">
         <v>7</v>
       </c>
       <c r="G58" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="59" spans="3:7">
@@ -2862,16 +2864,16 @@
         <v>61</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E59" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F59" s="10" t="s">
         <v>7</v>
       </c>
       <c r="G59" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="60" spans="3:7">
@@ -2879,16 +2881,16 @@
         <v>62</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E60" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F60" s="3" t="s">
         <v>7</v>
       </c>
       <c r="G60" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="61" spans="3:7">
@@ -2896,16 +2898,16 @@
         <v>63</v>
       </c>
       <c r="D61" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E61" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F61" s="3" t="s">
         <v>7</v>
       </c>
       <c r="G61" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="62" spans="3:7">
@@ -2913,21 +2915,21 @@
         <v>64</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F62" s="3" t="s">
         <v>7</v>
       </c>
       <c r="G62" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="63" spans="3:7">
       <c r="G63" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="65" spans="6:6">

</xml_diff>